<commit_message>
fixed province field data extraction
</commit_message>
<xml_diff>
--- a/src/invoices.xlsx
+++ b/src/invoices.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,25 +462,30 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Building</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>City</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Province</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Postal Code</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Agreement No</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Client Project</t>
         </is>
@@ -516,25 +521,30 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Stoney Creek</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>L8E 0J7</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>A0332</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>The Shores</t>
         </is>
@@ -568,27 +578,32 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A0212</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Origins - Additional Lots</t>
         </is>
       </c>
     </row>
@@ -620,25 +635,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Burlington</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>L7L 6A9</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>A0224</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Casa De Torri</t>
         </is>
@@ -672,25 +692,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Bldg. A</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Richmond Hill</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>L4B 1B9</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>A0178</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Urban North</t>
         </is>
@@ -724,25 +749,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Burlington</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>L7L 6A9</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>A0224</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Casa De Torri</t>
         </is>
@@ -776,25 +806,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>Bldg. A</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>Richmond Hill</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>L4B 1B9</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>A0178</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>Urban North</t>
         </is>
@@ -828,25 +863,30 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Burlington</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>L7L 6A9</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>A0224</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Casa De Torri</t>
         </is>
@@ -880,25 +920,30 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Burlington</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>L7L 6A9</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>A0224</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Casa De Torri</t>
         </is>
@@ -932,25 +977,30 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t>Bldg. A</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Richmond Hill</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>L4B 1B9</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>A0178</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Urban North</t>
         </is>
@@ -984,25 +1034,30 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Bldg. A</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Richmond Hill</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>L4B 1B9</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>A0178</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>Urban North</t>
         </is>
@@ -1036,25 +1091,30 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Stoney Creek</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Cr</t>
-        </is>
-      </c>
       <c r="H12" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>L8E 0J7</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1088,25 +1148,30 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>L4L 8A9</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>A0451</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>North West</t>
         </is>
@@ -1140,25 +1205,30 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H14" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>A0429-DE</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>GO Towns</t>
         </is>
@@ -1192,27 +1262,32 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A0456DE</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Whitby Meadows Phase 3</t>
         </is>
       </c>
     </row>
@@ -1244,25 +1319,30 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>Concord</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H16" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>L4K 5R2</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>A0426</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>Erin Glen</t>
         </is>
@@ -1296,27 +1376,32 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Barrie</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H17" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
           <t>L4M 0J4</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A0330</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Windfall Phase 4B</t>
         </is>
       </c>
     </row>
@@ -1348,25 +1433,30 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>A0504</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>Greenwood Seaton</t>
         </is>
@@ -1400,25 +1490,30 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>Concord</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H19" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
           <t>L4K 5R2</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>A0426</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>Erin Glen</t>
         </is>
@@ -1457,22 +1552,27 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Da</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
           <t>L4K 3Z9</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>A0501</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Fairway Meadows Phase 2</t>
         </is>
       </c>
     </row>
@@ -1504,25 +1604,30 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>A0546</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>Honeystone</t>
         </is>
@@ -1556,25 +1661,30 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H22" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>A0546</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>Honeystone</t>
         </is>
@@ -1608,25 +1718,30 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H23" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>A0546</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>Honeystone</t>
         </is>
@@ -1660,25 +1775,30 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Mississauga</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H24" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
           <t>L5N 6C3</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>A0521</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>Woodstock</t>
         </is>
@@ -1712,25 +1832,30 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>Mississauga</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H25" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
           <t>L5N 6C3</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>A0522</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>New Dundee Kitchener</t>
         </is>
@@ -1764,25 +1889,30 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>A0429-DE</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>GO Towns</t>
         </is>
@@ -1816,25 +1946,30 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>A0445</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>Seatonville</t>
         </is>
@@ -1868,25 +2003,30 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H28" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>A0464</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>Seaton South</t>
         </is>
@@ -1920,25 +2060,30 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H29" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>A0504</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>Greenwood Seaton</t>
         </is>
@@ -1972,25 +2117,30 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>Vaughan</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Da</t>
-        </is>
-      </c>
       <c r="H30" t="inlineStr">
         <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
           <t>L4K 4B4</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>A0546</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>Honeystone</t>
         </is>

</xml_diff>